<commit_message>
Added ScreenshotSaving to Document
</commit_message>
<xml_diff>
--- a/target/classes/CustomerAddressData.xlsx
+++ b/target/classes/CustomerAddressData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kpemmaraju\eclipse-workspace\TestNGProjectUsingTestListner\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F2D0C8-3740-4950-BFAC-34C09B5C437D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FED729-5475-4154-A7BB-0A440FF1C2AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1605" windowWidth="29040" windowHeight="15840" xr2:uid="{063F3F19-F1B0-4212-A3BE-0BB1634646FC}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>